<commit_message>
updated notes and spreadsaheet guidance for dicscipline property
</commit_message>
<xml_diff>
--- a/Journal_Comparison_Service_Data_Collection_FOAA-Based_v1.1.xlsx
+++ b/Journal_Comparison_Service_Data_Collection_FOAA-Based_v1.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulwalk/Dropbox/Reference/_ou/cOAlition S/PSTF/journal_comparison_service_data_collection_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD001DC-768E-9F4C-B72C-105412310FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2CD44E-AA64-F94D-8F92-32C252B25146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="33600" windowHeight="15640" xr2:uid="{64594A8F-0D25-2F4C-85DE-649BC0F5FC38}"/>
   </bookViews>
@@ -225,7 +225,25 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Numeric value from https://read.oecd-ilibrary.org/science-and-technology/frascati-manual-2015_9789264239012-en#page60 or one of the following:
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Enter value from https://read.oecd-ilibrary.org/science-and-technology/frascati-manual-2015_9789264239012-en#page60 (e.g. 1.6 Biological sciences) or one of the following</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">:
 </t>
         </r>
         <r>
@@ -2871,9 +2889,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A664604-316B-CC4E-8B2B-F0537DD1800C}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
updated guidance in spreadsheets and docs
</commit_message>
<xml_diff>
--- a/Journal_Comparison_Service_Data_Collection_FOAA-Based_v1.1.xlsx
+++ b/Journal_Comparison_Service_Data_Collection_FOAA-Based_v1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulwalk/Dropbox/Reference/_ou/cOAlition S/PSTF/journal_comparison_service_data_collection_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2CD44E-AA64-F94D-8F92-32C252B25146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A47E3BC-0E3F-E24B-AD6D-F00DEA4F5CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="33600" windowHeight="15640" xr2:uid="{64594A8F-0D25-2F4C-85DE-649BC0F5FC38}"/>
   </bookViews>
@@ -839,15 +839,24 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Subscription List Price Range Higher.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <scheme val="minor"/>
+          <t xml:space="preserve">Subscription List Price Range Higher. </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This should be the fee charged to an institution, not a personal subscriber.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t>This includes fees paid by libraries through models such as Subscribe to Open, Community Action Publishing, and library membership.</t>
         </r>
@@ -961,7 +970,36 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Subscription List Price Range Higher.
+          <t xml:space="preserve">Subscription List Price Range Higher. </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>This should be the fee charged to an institution, not a personal subscriber.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -1061,16 +1099,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">This is a required field. To facilitate comparison of list prices between publishers, please tell us the subscription list price for a typical research-intensive university in the US. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>If there is no subscription price, please enter 0.00</t>
+          <t>This is a required field. To facilitate comparison of list prices between publishers, please tell us the subscription list price for a typical research-intensive university in the US. If there is no subscription price, please enter 0.00</t>
         </r>
         <r>
           <rPr>
@@ -2389,7 +2418,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2481,6 +2510,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -2889,9 +2925,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A664604-316B-CC4E-8B2B-F0537DD1800C}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>